<commit_message>
Added new DB, Edited header and verified new connections to PHP file
</commit_message>
<xml_diff>
--- a/Template PSP.xlsx
+++ b/Template PSP.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DESKTOP\Google Drive\Backup HPE\Univa\9no\Calidad de software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Documents\NewsWebApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AB6C00B-6193-4A94-A181-74DEBC9A6BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D64775-F2D7-47E1-B3B4-6C06A7DA86A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{15B3A8AC-8F3B-479E-AEAE-8904FE888B03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15B3A8AC-8F3B-479E-AEAE-8904FE888B03}"/>
   </bookViews>
   <sheets>
-    <sheet name="Examen 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Emanuel - Semana 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Examen 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="61">
   <si>
     <t>Estudiante:</t>
   </si>
@@ -205,6 +206,18 @@
   </si>
   <si>
     <t>Tecnicos</t>
+  </si>
+  <si>
+    <t>PCS1</t>
+  </si>
+  <si>
+    <t>Dr. Edgar Cossio</t>
+  </si>
+  <si>
+    <t>Emanuel Camarena</t>
+  </si>
+  <si>
+    <t>1/Marzo/2021</t>
   </si>
 </sst>
 </file>
@@ -640,50 +653,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1688E8B3-5C85-46F7-A6FE-A0EAAA496E10}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A436740-C570-4BE1-A944-B305533011E3}">
   <dimension ref="B2:J76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:F32"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.3828125" customWidth="1"/>
-    <col min="4" max="4" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.3828125" customWidth="1"/>
-    <col min="7" max="7" width="14.15234375" customWidth="1"/>
-    <col min="8" max="8" width="28.3828125" customWidth="1"/>
-    <col min="9" max="9" width="11.53515625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3">
-        <v>35317</v>
+      <c r="G2" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -691,18 +704,18 @@
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:10" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:10" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
@@ -731,331 +744,153 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
-        <v>44448</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0.375</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="E8" s="10">
-        <v>1.3194444444444444E-2</v>
-      </c>
-      <c r="F8" s="11">
-        <f t="shared" ref="F8:F9" si="0">D8-C8-E8</f>
-        <v>2.1527777777777819E-2</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>18</v>
-      </c>
+        <v>44256</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
-      <c r="C9" s="9">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.5541666666666667</v>
-      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="11">
-        <f t="shared" si="0"/>
-        <v>2.6388888888888906E-2</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
-      <c r="C10" s="9">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0.66180555555555554</v>
-      </c>
-      <c r="E10" s="10">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="F10" s="11">
-        <f>D10-C10-E10</f>
-        <v>4.0277777777777718E-2</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
-      <c r="C11" s="9">
-        <v>0.76736111111111116</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0.82291666666666663</v>
-      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="11">
-        <f t="shared" ref="F11:F19" si="1">D11-C11-E11</f>
-        <v>5.5555555555555469E-2</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B12" s="8">
-        <v>44449</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0.46249999999999997</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0.5131944444444444</v>
-      </c>
-      <c r="E12" s="10">
-        <v>7.6388888888888886E-3</v>
-      </c>
-      <c r="F12" s="11">
-        <f t="shared" si="1"/>
-        <v>4.3055555555555541E-2</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B13" s="8">
-        <v>44450</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0.375</v>
-      </c>
-      <c r="D13" s="9">
-        <v>0.40972222222222227</v>
-      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="12"/>
-      <c r="F13" s="11">
-        <f t="shared" si="1"/>
-        <v>3.4722222222222265E-2</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
-      <c r="C14" s="9">
-        <v>0.55208333333333337</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.60763888888888895</v>
-      </c>
-      <c r="E14" s="10">
-        <v>7.6388888888888886E-3</v>
-      </c>
-      <c r="F14" s="11">
-        <f t="shared" si="1"/>
-        <v>4.7916666666666691E-2</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
-      <c r="C15" s="9">
-        <v>0.6791666666666667</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0.71597222222222223</v>
-      </c>
-      <c r="E15" s="10">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="F15" s="11">
-        <f t="shared" si="1"/>
-        <v>1.9444444444444424E-2</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B16" s="8">
-        <v>44451</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0.27916666666666667</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.37777777777777777</v>
-      </c>
-      <c r="E16" s="10">
-        <v>1.9444444444444445E-2</v>
-      </c>
-      <c r="F16" s="11">
-        <f t="shared" si="1"/>
-        <v>7.9166666666666649E-2</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B17" s="8">
-        <f>B16+1</f>
-        <v>44452</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0.375</v>
-      </c>
-      <c r="D17" s="9">
-        <v>0.40972222222222227</v>
-      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="11">
-        <f t="shared" si="1"/>
-        <v>3.4722222222222265E-2</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
-      <c r="C18" s="9">
-        <v>0.52638888888888891</v>
-      </c>
-      <c r="D18" s="9">
-        <v>0.55277777777777781</v>
-      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="11">
-        <f t="shared" si="1"/>
-        <v>2.6388888888888906E-2</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="8">
-        <f>B17+1</f>
-        <v>44453</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="D19" s="9">
-        <v>0.4993055555555555</v>
-      </c>
-      <c r="E19" s="10">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F19" s="11">
-        <f t="shared" si="1"/>
-        <v>9.3055555555555489E-2</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>30</v>
-      </c>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
       <c r="F20" s="16"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>31</v>
       </c>
@@ -1075,23 +910,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>40</v>
       </c>
@@ -1100,11 +929,11 @@
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17">
-        <f t="shared" ref="G26:G32" si="2">SUM(C26:F26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+        <f t="shared" ref="G26:G32" si="0">SUM(C26:F26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>41</v>
       </c>
@@ -1113,11 +942,11 @@
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>42</v>
       </c>
@@ -1126,11 +955,11 @@
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>43</v>
       </c>
@@ -1139,11 +968,11 @@
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>44</v>
       </c>
@@ -1152,11 +981,11 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="12" t="s">
         <v>45</v>
       </c>
@@ -1165,11 +994,11 @@
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
       <c r="G31" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>46</v>
       </c>
@@ -1178,11 +1007,11 @@
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>47</v>
       </c>
@@ -1191,15 +1020,15 @@
         <v>0</v>
       </c>
       <c r="D33" s="17">
-        <f t="shared" ref="D33:F33" si="3">SUM(D26:D32)</f>
+        <f t="shared" ref="D33:F33" si="1">SUM(D26:D32)</f>
         <v>0</v>
       </c>
       <c r="E33" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F33" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G33" s="17">
@@ -1208,12 +1037,12 @@
       </c>
       <c r="H33" s="18"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>36</v>
       </c>
@@ -1223,7 +1052,7 @@
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
         <v>49</v>
       </c>
@@ -1233,7 +1062,7 @@
       <c r="F38" s="12"/>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
         <v>50</v>
       </c>
@@ -1243,7 +1072,7 @@
       <c r="F39" s="12"/>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
         <v>51</v>
       </c>
@@ -1253,12 +1082,12 @@
       <c r="F40" s="12"/>
       <c r="G40" s="17"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
         <v>36</v>
       </c>
@@ -1268,7 +1097,7 @@
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
         <v>49</v>
       </c>
@@ -1278,7 +1107,7 @@
       <c r="F45" s="12"/>
       <c r="G45" s="17"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
         <v>50</v>
       </c>
@@ -1288,7 +1117,7 @@
       <c r="F46" s="12"/>
       <c r="G46" s="17"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
         <v>51</v>
       </c>
@@ -1298,12 +1127,12 @@
       <c r="F47" s="12"/>
       <c r="G47" s="17"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
         <v>31</v>
       </c>
@@ -1329,27 +1158,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>56</v>
-      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
       <c r="G54" s="12"/>
-      <c r="H54" s="12" t="s">
-        <v>39</v>
-      </c>
+      <c r="H54" s="12"/>
       <c r="I54" s="12"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="12" t="s">
         <v>40</v>
       </c>
@@ -1361,7 +1182,7 @@
       <c r="H55" s="20"/>
       <c r="I55" s="20"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="12" t="s">
         <v>41</v>
       </c>
@@ -1373,7 +1194,7 @@
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="12" t="s">
         <v>42</v>
       </c>
@@ -1385,7 +1206,7 @@
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="12" t="s">
         <v>43</v>
       </c>
@@ -1397,7 +1218,7 @@
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="12" t="s">
         <v>44</v>
       </c>
@@ -1409,7 +1230,7 @@
       <c r="H59" s="20"/>
       <c r="I59" s="20"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="12" t="s">
         <v>45</v>
       </c>
@@ -1421,7 +1242,7 @@
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="12" t="s">
         <v>46</v>
       </c>
@@ -1433,7 +1254,7 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="12" t="s">
         <v>47</v>
       </c>
@@ -1442,23 +1263,23 @@
         <v>0</v>
       </c>
       <c r="D62" s="20">
-        <f t="shared" ref="D62:H62" si="4">SUM(D55:D61)</f>
+        <f t="shared" ref="D62:H62" si="2">SUM(D55:D61)</f>
         <v>0</v>
       </c>
       <c r="E62" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F62" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G62" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H62" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I62" s="20">
@@ -1466,12 +1287,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="12" t="s">
         <v>36</v>
       </c>
@@ -1483,7 +1304,7 @@
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="12" t="s">
         <v>49</v>
       </c>
@@ -1495,7 +1316,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="12" t="s">
         <v>50</v>
       </c>
@@ -1507,7 +1328,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="12"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="12" t="s">
         <v>51</v>
       </c>
@@ -1519,12 +1340,12 @@
       <c r="H69" s="12"/>
       <c r="I69" s="12"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="12" t="s">
         <v>36</v>
       </c>
@@ -1539,7 +1360,954 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="17">
+        <f t="shared" ref="I74:I76" si="3">SUM(C74:H74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1688E8B3-5C85-46F7-A6FE-A0EAAA496E10}">
+  <dimension ref="B2:J76"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>35317</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="7" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>44448</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" ref="F8:F9" si="0">D8-C8-E8</f>
+        <v>2.1527777777777819E-2</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="9">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>2.6388888888888906E-2</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="9">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.66180555555555554</v>
+      </c>
+      <c r="E10" s="10">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F10" s="11">
+        <f>D10-C10-E10</f>
+        <v>4.0277777777777718E-2</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+      <c r="C11" s="9">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11">
+        <f t="shared" ref="F11:F19" si="1">D11-C11-E11</f>
+        <v>5.5555555555555469E-2</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>44449</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.5131944444444444</v>
+      </c>
+      <c r="E12" s="10">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="1"/>
+        <v>4.3055555555555541E-2</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>44450</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11">
+        <f t="shared" si="1"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="9">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="E14" s="10">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="1"/>
+        <v>4.7916666666666691E-2</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="9">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="1"/>
+        <v>1.9444444444444424E-2</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>44451</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0.27916666666666667</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="1"/>
+        <v>7.9166666666666649E-2</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <f>B16+1</f>
+        <v>44452</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="11">
+        <f t="shared" si="1"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="9">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="11">
+        <f t="shared" si="1"/>
+        <v>2.6388888888888906E-2</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <f>B17+1</f>
+        <v>44453</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="E19" s="10">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="1"/>
+        <v>9.3055555555555489E-2</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17">
+        <f t="shared" ref="G26:G32" si="2">SUM(C26:F26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="17">
+        <f>SUM(C26:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="17">
+        <f t="shared" ref="D33:F33" si="3">SUM(D26:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="17">
+        <f>SUM(G26:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="17"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="17"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="17"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="17"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" s="12"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" s="20">
+        <f>SUM(C55:C61)</f>
+        <v>0</v>
+      </c>
+      <c r="D62" s="20">
+        <f t="shared" ref="D62:H62" si="4">SUM(D55:D61)</f>
+        <v>0</v>
+      </c>
+      <c r="E62" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I62" s="20">
+        <f>SUM(I55:I61)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17">
+        <f>SUM(C73:H73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="12" t="s">
         <v>49</v>
       </c>
@@ -1554,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="12" t="s">
         <v>50</v>
       </c>
@@ -1569,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="12" t="s">
         <v>51</v>
       </c>

</xml_diff>